<commit_message>
made minor improvements to portfolio piece
</commit_message>
<xml_diff>
--- a/files/portfolio/data-analysis/us-bank-failures-since-2000.xlsx
+++ b/files/portfolio/data-analysis/us-bank-failures-since-2000.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alienware\Desktop\data-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alienware\Documents\jakel1828.github.io\files\portfolio\data-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBDA634-CB1A-42BC-9356-0DAB95D4A043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B108638-366A-4C58-9BA0-5AEE8633BE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4190,7 +4190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4208,6 +4208,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5555,11 +5556,11 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -5621,9 +5622,8 @@
           <c:h val="0.50711827661360787"/>
         </c:manualLayout>
       </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -5640,76 +5640,78 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>'scratch by year'!$A$4:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2010</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>2011</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="10">
                   <c:v>2012</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="11">
                   <c:v>2013</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12">
                   <c:v>2014</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>2002</c:v>
+                <c:pt idx="13">
+                  <c:v>2015</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="14">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>2017</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>2015</c:v>
+                <c:pt idx="16">
+                  <c:v>2019</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="17">
                   <c:v>2020</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2003</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>2000</c:v>
+                  <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2024</c:v>
@@ -5727,61 +5729,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>157</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>92</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="10">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="11">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="16">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="17">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2</c:v>
@@ -5792,6 +5794,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9765-4D81-8D95-DBE49791C298}"/>
@@ -5806,11 +5809,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:smooth val="0"/>
         <c:axId val="683347112"/>
         <c:axId val="683346328"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="683347112"/>
         <c:scaling>
@@ -8876,15 +8878,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23682,6 +23684,243 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000002000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="A1:B41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" measureFilter="1" sortType="descending">
+      <items count="45">
+        <item x="33"/>
+        <item x="17"/>
+        <item x="29"/>
+        <item x="5"/>
+        <item x="21"/>
+        <item x="28"/>
+        <item x="7"/>
+        <item x="18"/>
+        <item x="43"/>
+        <item x="3"/>
+        <item x="27"/>
+        <item x="0"/>
+        <item x="35"/>
+        <item x="4"/>
+        <item x="12"/>
+        <item x="15"/>
+        <item x="39"/>
+        <item x="24"/>
+        <item x="34"/>
+        <item x="23"/>
+        <item x="32"/>
+        <item x="36"/>
+        <item x="31"/>
+        <item x="9"/>
+        <item x="42"/>
+        <item x="10"/>
+        <item x="37"/>
+        <item x="30"/>
+        <item x="6"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="38"/>
+        <item x="2"/>
+        <item x="22"/>
+        <item x="25"/>
+        <item x="40"/>
+        <item x="19"/>
+        <item x="13"/>
+        <item x="16"/>
+        <item x="26"/>
+        <item x="20"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="41"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="14" showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="40">
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Closing Date " fld="6" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="2" type="valueGreaterThan" evalOrder="-1" id="2" iMeasureFld="0">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter operator="greaterThan" val="1"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+  </filters>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000001000000}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Total" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="G1:H12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
@@ -24233,7 +24472,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
@@ -24348,245 +24587,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000002000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
-  <location ref="A1:B41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" measureFilter="1" sortType="descending">
-      <items count="45">
-        <item x="33"/>
-        <item x="17"/>
-        <item x="29"/>
-        <item x="5"/>
-        <item x="21"/>
-        <item x="28"/>
-        <item x="7"/>
-        <item x="18"/>
-        <item x="43"/>
-        <item x="3"/>
-        <item x="27"/>
-        <item x="0"/>
-        <item x="35"/>
-        <item x="4"/>
-        <item x="12"/>
-        <item x="15"/>
-        <item x="39"/>
-        <item x="24"/>
-        <item x="34"/>
-        <item x="23"/>
-        <item x="32"/>
-        <item x="36"/>
-        <item x="31"/>
-        <item x="9"/>
-        <item x="42"/>
-        <item x="10"/>
-        <item x="37"/>
-        <item x="30"/>
-        <item x="6"/>
-        <item x="11"/>
-        <item x="1"/>
-        <item x="38"/>
-        <item x="2"/>
-        <item x="22"/>
-        <item x="25"/>
-        <item x="40"/>
-        <item x="19"/>
-        <item x="13"/>
-        <item x="16"/>
-        <item x="26"/>
-        <item x="20"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="41"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="14" showAll="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="40">
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Closing Date " fld="6" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="1">
-    <filter fld="2" type="valueGreaterThan" evalOrder="-1" id="2" iMeasureFld="0">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <customFilters>
-            <customFilter operator="greaterThan" val="1"/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
-    </filter>
-  </filters>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0500-000003000000}" name="PivotTable14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0500-000003000000}" name="PivotTable14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
   <location ref="A3:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -24597,7 +24599,7 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
       <items count="22">
         <item x="20"/>
         <item x="19"/>
@@ -24622,15 +24624,6 @@
         <item x="0"/>
         <item t="default"/>
       </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -24640,10 +24633,31 @@
   </rowFields>
   <rowItems count="22">
     <i>
-      <x v="8"/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
     </i>
     <i>
       <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
     </i>
     <i>
       <x v="9"/>
@@ -24652,19 +24666,10 @@
       <x v="10"/>
     </i>
     <i>
-      <x v="6"/>
-    </i>
-    <i>
       <x v="11"/>
     </i>
     <i>
       <x v="12"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="15"/>
     </i>
     <i>
       <x v="13"/>
@@ -24673,28 +24678,16 @@
       <x v="14"/>
     </i>
     <i>
-      <x v="18"/>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
     </i>
     <i>
       <x v="17"/>
     </i>
     <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x/>
+      <x v="18"/>
     </i>
     <i>
       <x v="19"/>
@@ -25748,7 +25741,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25802,7 +25795,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="T21" sqref="T20:T21"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27000,7 +26993,7 @@
   <dimension ref="A3:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27038,10 +27031,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>1355</v>
-      </c>
-      <c r="B4">
-        <v>157</v>
+        <v>1347</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>1355</v>
@@ -27058,10 +27051,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>1354</v>
-      </c>
-      <c r="B5">
-        <v>140</v>
+        <v>1348</v>
+      </c>
+      <c r="B5" s="9">
+        <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>1354</v>
@@ -27078,10 +27071,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>1356</v>
-      </c>
-      <c r="B6">
-        <v>92</v>
+        <v>1349</v>
+      </c>
+      <c r="B6" s="9">
+        <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>1356</v>
@@ -27098,10 +27091,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>1357</v>
-      </c>
-      <c r="B7">
-        <v>51</v>
+        <v>1350</v>
+      </c>
+      <c r="B7" s="9">
+        <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>1357</v>
@@ -27118,10 +27111,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B8">
-        <v>25</v>
+        <v>1351</v>
+      </c>
+      <c r="B8" s="9">
+        <v>4</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>1353</v>
@@ -27138,10 +27131,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>1358</v>
-      </c>
-      <c r="B9">
-        <v>24</v>
+        <v>1352</v>
+      </c>
+      <c r="B9" s="9">
+        <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>1358</v>
@@ -27158,10 +27151,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>1359</v>
-      </c>
-      <c r="B10">
-        <v>18</v>
+        <v>1353</v>
+      </c>
+      <c r="B10" s="9">
+        <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>1359</v>
@@ -27178,10 +27171,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>1349</v>
-      </c>
-      <c r="B11">
-        <v>11</v>
+        <v>1354</v>
+      </c>
+      <c r="B11" s="9">
+        <v>140</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>1331</v>
@@ -27198,10 +27191,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>1362</v>
-      </c>
-      <c r="B12">
-        <v>8</v>
+        <v>1355</v>
+      </c>
+      <c r="B12" s="9">
+        <v>157</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>1348</v>
@@ -27212,10 +27205,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>1360</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
+        <v>1356</v>
+      </c>
+      <c r="B13" s="9">
+        <v>92</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>1352</v>
@@ -27226,10 +27219,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>1361</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
+        <v>1357</v>
+      </c>
+      <c r="B14" s="9">
+        <v>51</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>1350</v>
@@ -27240,10 +27233,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>1365</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
+        <v>1358</v>
+      </c>
+      <c r="B15" s="9">
+        <v>24</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>1347</v>
@@ -27254,10 +27247,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>1364</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
+        <v>1359</v>
+      </c>
+      <c r="B16" s="9">
+        <v>18</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>1366</v>
@@ -27268,10 +27261,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>1363</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
+        <v>1360</v>
+      </c>
+      <c r="B17" s="9">
+        <v>8</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>1367</v>
@@ -27282,10 +27275,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>1351</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
+        <v>1361</v>
+      </c>
+      <c r="B18" s="9">
+        <v>5</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>1331</v>
@@ -27296,41 +27289,41 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>1348</v>
-      </c>
-      <c r="B19">
-        <v>4</v>
+        <v>1362</v>
+      </c>
+      <c r="B19" s="9">
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>1352</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
+        <v>1363</v>
+      </c>
+      <c r="B20" s="9">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>1350</v>
-      </c>
-      <c r="B21">
-        <v>3</v>
+        <v>1364</v>
+      </c>
+      <c r="B21" s="9">
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
+        <v>1365</v>
+      </c>
+      <c r="B22" s="9">
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>1366</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="9">
         <v>2</v>
       </c>
     </row>
@@ -27338,7 +27331,7 @@
       <c r="A24" s="5" t="s">
         <v>1367</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="9">
         <v>1</v>
       </c>
     </row>
@@ -27346,7 +27339,7 @@
       <c r="A25" s="5" t="s">
         <v>1331</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="9">
         <v>571</v>
       </c>
     </row>
@@ -47543,7 +47536,7 @@
   <dimension ref="A1:G572"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="G1" sqref="A1:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>